<commit_message>
feat: update test account register
</commit_message>
<xml_diff>
--- a/Report/Đăng ký tài khoản.xlsx
+++ b/Report/Đăng ký tài khoản.xlsx
@@ -252,12 +252,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
       <t>Format: A@B
 Length: Trong vòng 100 ký tự
 Trong đó,
@@ -586,7 +580,7 @@
 Trường hợp:
 Confirm thành công, hiển thị [MMA-010-Homepage] với dialog xin quyền vị trí nếu lần đầu đăng nhập
 Confirm thất bại: 
-            Confirm code hết hạn, hiển thị [Mã OTP đã hết hạn (\n) Vui lòng gửi lại mã xác minh], tô đỏ field confirm code, disable [xác nhận] button 
+            Confirm code hết hạn, hiển thị [Mã xác minh đã hết hạn (\n) Vui lòng gửi lại mã xác minh], tô đỏ field confirm code, disable [xác nhận] button 
             Confirm code không đúng, hiển thị [Mã xác minh không chính xác], tô đỏ field confirm code, disable [xác nhận] button 
 Các case thất bại khác, hiển thị [Đã xảy ra lỗi. Vui lòng kiểm tra và thử lại.]. Click button OK trên message hiển thị màn hình [MMA-008-Confirm code] và confirm code được clear </t>
   </si>
@@ -9746,8 +9740,8 @@
   <sheetPr/>
   <dimension ref="A1:AB323"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="25" topLeftCell="G137" workbookViewId="0">
+      <selection activeCell="H151" sqref="H151:H164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
update result test register account
</commit_message>
<xml_diff>
--- a/Report/Đăng ký tài khoản.xlsx
+++ b/Report/Đăng ký tài khoản.xlsx
@@ -252,6 +252,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Format: A@B
 Length: Trong vòng 100 ký tự
 Trong đó,
@@ -9740,8 +9746,8 @@
   <sheetPr/>
   <dimension ref="A1:AB323"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="25" topLeftCell="G137" workbookViewId="0">
-      <selection activeCell="H151" sqref="H151:H164"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="25" topLeftCell="E179" workbookViewId="0">
+      <selection activeCell="O189" sqref="O189:O191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>

</xml_diff>